<commit_message>
Add selection-compare excel sheet
</commit_message>
<xml_diff>
--- a/data/code_size.xlsx
+++ b/data/code_size.xlsx
@@ -464,7 +464,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Binary Size Increase (Bytes)</a:t>
+                  <a:t>Binary Size per</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Version</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> (Bytes)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -473,8 +481,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.1904761904761904E-2"/>
-              <c:y val="9.184579866780615E-2"/>
+              <c:x val="8.9285714285714281E-3"/>
+              <c:y val="5.1779027727046789E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1494,7 +1502,7 @@
   <dimension ref="D5:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>